<commit_message>
Collected the excel tables for estimation of sustainable fisheries per species and municipality (landings data, ICES stocks data, municipalities codes, sea area).
</commit_message>
<xml_diff>
--- a/prep/food_provision/Fisheries/data/ices_bmsy.xlsx
+++ b/prep/food_provision/Fisheries/data/ices_bmsy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/Documents/Marina/Research/Postdoc  HI/OHI goals data and log /Food production /Fisheries data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marinaespinasse/github/nor-prep/prep/food_provision/Fisheries/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF9734D0-5982-2C42-9587-2A06ED4784CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E1B7EC-708B-E44E-8BBB-C5EF26696FD6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="1060" windowWidth="33540" windowHeight="19120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1000" yWindow="7900" windowWidth="33540" windowHeight="19120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SSB and Bmsy data" sheetId="1" r:id="rId1"/>
@@ -128,7 +128,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -138,6 +138,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -154,10 +160,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,15 +447,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N80"/>
   <sheetViews>
-    <sheetView zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3:M4"/>
+    <sheetView tabSelected="1" zoomScale="158" zoomScaleNormal="158" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="12" max="12" width="12.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -567,7 +574,7 @@
       <c r="B8" t="s">
         <v>9</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D8" t="s">
@@ -576,13 +583,13 @@
       <c r="E8" t="s">
         <v>9</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="G8" t="s">
         <v>9</v>
       </c>
-      <c r="H8" t="s">
+      <c r="H8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I8" t="s">
@@ -594,10 +601,10 @@
       <c r="K8" t="s">
         <v>9</v>
       </c>
-      <c r="L8" t="s">
+      <c r="L8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N8" t="s">
+      <c r="N8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
@@ -959,7 +966,7 @@
         <v>0.61767608695652176</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
+        <f>IF(B19&lt;$B$6,0,1)</f>
         <v>1</v>
       </c>
       <c r="E19" s="1">
@@ -3489,7 +3496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V145"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>

</xml_diff>